<commit_message>
Templates: colonnes Prénom et Nom séparées (comme anciens templates)
</commit_message>
<xml_diff>
--- a/template_greve.xlsx
+++ b/template_greve.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K156"/>
+  <dimension ref="A1:L156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,8 +469,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
@@ -480,6 +480,7 @@
     <col width="8" customWidth="1" min="9" max="9"/>
     <col width="8" customWidth="1" min="10" max="10"/>
     <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -499,63 +500,68 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Enseignant</t>
+          <t>Prénom</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>Nom</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>P3</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>P4</t>
+          <t>P3</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>P5</t>
+          <t>P4</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
         <is>
-          <t>P6</t>
+          <t>P5</t>
         </is>
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>P7</t>
+          <t>P6</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>P7</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr">
         <is>
-          <t>P9</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="K4" s="3" t="inlineStr">
         <is>
+          <t>P9</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="inlineStr">
+        <is>
           <t>P10</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="n"/>
-      <c r="B5" s="5" t="n"/>
+      <c r="B5" s="4" t="n"/>
       <c r="C5" s="5" t="n"/>
       <c r="D5" s="5" t="n"/>
       <c r="E5" s="5" t="n"/>
@@ -565,10 +571,11 @@
       <c r="I5" s="5" t="n"/>
       <c r="J5" s="5" t="n"/>
       <c r="K5" s="5" t="n"/>
+      <c r="L5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n"/>
-      <c r="B6" s="5" t="n"/>
+      <c r="B6" s="4" t="n"/>
       <c r="C6" s="5" t="n"/>
       <c r="D6" s="5" t="n"/>
       <c r="E6" s="5" t="n"/>
@@ -578,10 +585,11 @@
       <c r="I6" s="5" t="n"/>
       <c r="J6" s="5" t="n"/>
       <c r="K6" s="5" t="n"/>
+      <c r="L6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="n"/>
-      <c r="B7" s="5" t="n"/>
+      <c r="B7" s="4" t="n"/>
       <c r="C7" s="5" t="n"/>
       <c r="D7" s="5" t="n"/>
       <c r="E7" s="5" t="n"/>
@@ -591,10 +599,11 @@
       <c r="I7" s="5" t="n"/>
       <c r="J7" s="5" t="n"/>
       <c r="K7" s="5" t="n"/>
+      <c r="L7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n"/>
-      <c r="B8" s="5" t="n"/>
+      <c r="B8" s="4" t="n"/>
       <c r="C8" s="5" t="n"/>
       <c r="D8" s="5" t="n"/>
       <c r="E8" s="5" t="n"/>
@@ -604,10 +613,11 @@
       <c r="I8" s="5" t="n"/>
       <c r="J8" s="5" t="n"/>
       <c r="K8" s="5" t="n"/>
+      <c r="L8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="n"/>
-      <c r="B9" s="5" t="n"/>
+      <c r="B9" s="4" t="n"/>
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
       <c r="E9" s="5" t="n"/>
@@ -617,10 +627,11 @@
       <c r="I9" s="5" t="n"/>
       <c r="J9" s="5" t="n"/>
       <c r="K9" s="5" t="n"/>
+      <c r="L9" s="5" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="n"/>
-      <c r="B10" s="5" t="n"/>
+      <c r="B10" s="4" t="n"/>
       <c r="C10" s="5" t="n"/>
       <c r="D10" s="5" t="n"/>
       <c r="E10" s="5" t="n"/>
@@ -630,10 +641,11 @@
       <c r="I10" s="5" t="n"/>
       <c r="J10" s="5" t="n"/>
       <c r="K10" s="5" t="n"/>
+      <c r="L10" s="5" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="n"/>
-      <c r="B11" s="5" t="n"/>
+      <c r="B11" s="4" t="n"/>
       <c r="C11" s="5" t="n"/>
       <c r="D11" s="5" t="n"/>
       <c r="E11" s="5" t="n"/>
@@ -643,10 +655,11 @@
       <c r="I11" s="5" t="n"/>
       <c r="J11" s="5" t="n"/>
       <c r="K11" s="5" t="n"/>
+      <c r="L11" s="5" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="4" t="n"/>
-      <c r="B12" s="5" t="n"/>
+      <c r="B12" s="4" t="n"/>
       <c r="C12" s="5" t="n"/>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="5" t="n"/>
@@ -656,10 +669,11 @@
       <c r="I12" s="5" t="n"/>
       <c r="J12" s="5" t="n"/>
       <c r="K12" s="5" t="n"/>
+      <c r="L12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n"/>
-      <c r="B13" s="5" t="n"/>
+      <c r="B13" s="4" t="n"/>
       <c r="C13" s="5" t="n"/>
       <c r="D13" s="5" t="n"/>
       <c r="E13" s="5" t="n"/>
@@ -669,10 +683,11 @@
       <c r="I13" s="5" t="n"/>
       <c r="J13" s="5" t="n"/>
       <c r="K13" s="5" t="n"/>
+      <c r="L13" s="5" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="n"/>
-      <c r="B14" s="5" t="n"/>
+      <c r="B14" s="4" t="n"/>
       <c r="C14" s="5" t="n"/>
       <c r="D14" s="5" t="n"/>
       <c r="E14" s="5" t="n"/>
@@ -682,10 +697,11 @@
       <c r="I14" s="5" t="n"/>
       <c r="J14" s="5" t="n"/>
       <c r="K14" s="5" t="n"/>
+      <c r="L14" s="5" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n"/>
-      <c r="B15" s="5" t="n"/>
+      <c r="B15" s="4" t="n"/>
       <c r="C15" s="5" t="n"/>
       <c r="D15" s="5" t="n"/>
       <c r="E15" s="5" t="n"/>
@@ -695,10 +711,11 @@
       <c r="I15" s="5" t="n"/>
       <c r="J15" s="5" t="n"/>
       <c r="K15" s="5" t="n"/>
+      <c r="L15" s="5" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n"/>
-      <c r="B16" s="5" t="n"/>
+      <c r="B16" s="4" t="n"/>
       <c r="C16" s="5" t="n"/>
       <c r="D16" s="5" t="n"/>
       <c r="E16" s="5" t="n"/>
@@ -708,10 +725,11 @@
       <c r="I16" s="5" t="n"/>
       <c r="J16" s="5" t="n"/>
       <c r="K16" s="5" t="n"/>
+      <c r="L16" s="5" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n"/>
-      <c r="B17" s="5" t="n"/>
+      <c r="B17" s="4" t="n"/>
       <c r="C17" s="5" t="n"/>
       <c r="D17" s="5" t="n"/>
       <c r="E17" s="5" t="n"/>
@@ -721,10 +739,11 @@
       <c r="I17" s="5" t="n"/>
       <c r="J17" s="5" t="n"/>
       <c r="K17" s="5" t="n"/>
+      <c r="L17" s="5" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="n"/>
-      <c r="B18" s="5" t="n"/>
+      <c r="B18" s="4" t="n"/>
       <c r="C18" s="5" t="n"/>
       <c r="D18" s="5" t="n"/>
       <c r="E18" s="5" t="n"/>
@@ -734,10 +753,11 @@
       <c r="I18" s="5" t="n"/>
       <c r="J18" s="5" t="n"/>
       <c r="K18" s="5" t="n"/>
+      <c r="L18" s="5" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n"/>
-      <c r="B19" s="5" t="n"/>
+      <c r="B19" s="4" t="n"/>
       <c r="C19" s="5" t="n"/>
       <c r="D19" s="5" t="n"/>
       <c r="E19" s="5" t="n"/>
@@ -747,10 +767,11 @@
       <c r="I19" s="5" t="n"/>
       <c r="J19" s="5" t="n"/>
       <c r="K19" s="5" t="n"/>
+      <c r="L19" s="5" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="4" t="n"/>
-      <c r="B20" s="5" t="n"/>
+      <c r="B20" s="4" t="n"/>
       <c r="C20" s="5" t="n"/>
       <c r="D20" s="5" t="n"/>
       <c r="E20" s="5" t="n"/>
@@ -760,10 +781,11 @@
       <c r="I20" s="5" t="n"/>
       <c r="J20" s="5" t="n"/>
       <c r="K20" s="5" t="n"/>
+      <c r="L20" s="5" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n"/>
-      <c r="B21" s="5" t="n"/>
+      <c r="B21" s="4" t="n"/>
       <c r="C21" s="5" t="n"/>
       <c r="D21" s="5" t="n"/>
       <c r="E21" s="5" t="n"/>
@@ -773,10 +795,11 @@
       <c r="I21" s="5" t="n"/>
       <c r="J21" s="5" t="n"/>
       <c r="K21" s="5" t="n"/>
+      <c r="L21" s="5" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="4" t="n"/>
-      <c r="B22" s="5" t="n"/>
+      <c r="B22" s="4" t="n"/>
       <c r="C22" s="5" t="n"/>
       <c r="D22" s="5" t="n"/>
       <c r="E22" s="5" t="n"/>
@@ -786,10 +809,11 @@
       <c r="I22" s="5" t="n"/>
       <c r="J22" s="5" t="n"/>
       <c r="K22" s="5" t="n"/>
+      <c r="L22" s="5" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n"/>
-      <c r="B23" s="5" t="n"/>
+      <c r="B23" s="4" t="n"/>
       <c r="C23" s="5" t="n"/>
       <c r="D23" s="5" t="n"/>
       <c r="E23" s="5" t="n"/>
@@ -799,10 +823,11 @@
       <c r="I23" s="5" t="n"/>
       <c r="J23" s="5" t="n"/>
       <c r="K23" s="5" t="n"/>
+      <c r="L23" s="5" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="4" t="n"/>
-      <c r="B24" s="5" t="n"/>
+      <c r="B24" s="4" t="n"/>
       <c r="C24" s="5" t="n"/>
       <c r="D24" s="5" t="n"/>
       <c r="E24" s="5" t="n"/>
@@ -812,10 +837,11 @@
       <c r="I24" s="5" t="n"/>
       <c r="J24" s="5" t="n"/>
       <c r="K24" s="5" t="n"/>
+      <c r="L24" s="5" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n"/>
-      <c r="B25" s="5" t="n"/>
+      <c r="B25" s="4" t="n"/>
       <c r="C25" s="5" t="n"/>
       <c r="D25" s="5" t="n"/>
       <c r="E25" s="5" t="n"/>
@@ -825,10 +851,11 @@
       <c r="I25" s="5" t="n"/>
       <c r="J25" s="5" t="n"/>
       <c r="K25" s="5" t="n"/>
+      <c r="L25" s="5" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n"/>
-      <c r="B26" s="5" t="n"/>
+      <c r="B26" s="4" t="n"/>
       <c r="C26" s="5" t="n"/>
       <c r="D26" s="5" t="n"/>
       <c r="E26" s="5" t="n"/>
@@ -838,10 +865,11 @@
       <c r="I26" s="5" t="n"/>
       <c r="J26" s="5" t="n"/>
       <c r="K26" s="5" t="n"/>
+      <c r="L26" s="5" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="n"/>
-      <c r="B27" s="5" t="n"/>
+      <c r="B27" s="4" t="n"/>
       <c r="C27" s="5" t="n"/>
       <c r="D27" s="5" t="n"/>
       <c r="E27" s="5" t="n"/>
@@ -851,10 +879,11 @@
       <c r="I27" s="5" t="n"/>
       <c r="J27" s="5" t="n"/>
       <c r="K27" s="5" t="n"/>
+      <c r="L27" s="5" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="4" t="n"/>
-      <c r="B28" s="5" t="n"/>
+      <c r="B28" s="4" t="n"/>
       <c r="C28" s="5" t="n"/>
       <c r="D28" s="5" t="n"/>
       <c r="E28" s="5" t="n"/>
@@ -864,10 +893,11 @@
       <c r="I28" s="5" t="n"/>
       <c r="J28" s="5" t="n"/>
       <c r="K28" s="5" t="n"/>
+      <c r="L28" s="5" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="n"/>
-      <c r="B29" s="5" t="n"/>
+      <c r="B29" s="4" t="n"/>
       <c r="C29" s="5" t="n"/>
       <c r="D29" s="5" t="n"/>
       <c r="E29" s="5" t="n"/>
@@ -877,10 +907,11 @@
       <c r="I29" s="5" t="n"/>
       <c r="J29" s="5" t="n"/>
       <c r="K29" s="5" t="n"/>
+      <c r="L29" s="5" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="4" t="n"/>
-      <c r="B30" s="5" t="n"/>
+      <c r="B30" s="4" t="n"/>
       <c r="C30" s="5" t="n"/>
       <c r="D30" s="5" t="n"/>
       <c r="E30" s="5" t="n"/>
@@ -890,10 +921,11 @@
       <c r="I30" s="5" t="n"/>
       <c r="J30" s="5" t="n"/>
       <c r="K30" s="5" t="n"/>
+      <c r="L30" s="5" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="n"/>
-      <c r="B31" s="5" t="n"/>
+      <c r="B31" s="4" t="n"/>
       <c r="C31" s="5" t="n"/>
       <c r="D31" s="5" t="n"/>
       <c r="E31" s="5" t="n"/>
@@ -903,10 +935,11 @@
       <c r="I31" s="5" t="n"/>
       <c r="J31" s="5" t="n"/>
       <c r="K31" s="5" t="n"/>
+      <c r="L31" s="5" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="n"/>
-      <c r="B32" s="5" t="n"/>
+      <c r="B32" s="4" t="n"/>
       <c r="C32" s="5" t="n"/>
       <c r="D32" s="5" t="n"/>
       <c r="E32" s="5" t="n"/>
@@ -916,10 +949,11 @@
       <c r="I32" s="5" t="n"/>
       <c r="J32" s="5" t="n"/>
       <c r="K32" s="5" t="n"/>
+      <c r="L32" s="5" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="4" t="n"/>
-      <c r="B33" s="5" t="n"/>
+      <c r="B33" s="4" t="n"/>
       <c r="C33" s="5" t="n"/>
       <c r="D33" s="5" t="n"/>
       <c r="E33" s="5" t="n"/>
@@ -929,10 +963,11 @@
       <c r="I33" s="5" t="n"/>
       <c r="J33" s="5" t="n"/>
       <c r="K33" s="5" t="n"/>
+      <c r="L33" s="5" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="n"/>
-      <c r="B34" s="5" t="n"/>
+      <c r="B34" s="4" t="n"/>
       <c r="C34" s="5" t="n"/>
       <c r="D34" s="5" t="n"/>
       <c r="E34" s="5" t="n"/>
@@ -942,10 +977,11 @@
       <c r="I34" s="5" t="n"/>
       <c r="J34" s="5" t="n"/>
       <c r="K34" s="5" t="n"/>
+      <c r="L34" s="5" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="n"/>
-      <c r="B35" s="5" t="n"/>
+      <c r="B35" s="4" t="n"/>
       <c r="C35" s="5" t="n"/>
       <c r="D35" s="5" t="n"/>
       <c r="E35" s="5" t="n"/>
@@ -955,10 +991,11 @@
       <c r="I35" s="5" t="n"/>
       <c r="J35" s="5" t="n"/>
       <c r="K35" s="5" t="n"/>
+      <c r="L35" s="5" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="n"/>
-      <c r="B36" s="5" t="n"/>
+      <c r="B36" s="4" t="n"/>
       <c r="C36" s="5" t="n"/>
       <c r="D36" s="5" t="n"/>
       <c r="E36" s="5" t="n"/>
@@ -968,10 +1005,11 @@
       <c r="I36" s="5" t="n"/>
       <c r="J36" s="5" t="n"/>
       <c r="K36" s="5" t="n"/>
+      <c r="L36" s="5" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="n"/>
-      <c r="B37" s="5" t="n"/>
+      <c r="B37" s="4" t="n"/>
       <c r="C37" s="5" t="n"/>
       <c r="D37" s="5" t="n"/>
       <c r="E37" s="5" t="n"/>
@@ -981,10 +1019,11 @@
       <c r="I37" s="5" t="n"/>
       <c r="J37" s="5" t="n"/>
       <c r="K37" s="5" t="n"/>
+      <c r="L37" s="5" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="n"/>
-      <c r="B38" s="5" t="n"/>
+      <c r="B38" s="4" t="n"/>
       <c r="C38" s="5" t="n"/>
       <c r="D38" s="5" t="n"/>
       <c r="E38" s="5" t="n"/>
@@ -994,10 +1033,11 @@
       <c r="I38" s="5" t="n"/>
       <c r="J38" s="5" t="n"/>
       <c r="K38" s="5" t="n"/>
+      <c r="L38" s="5" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="4" t="n"/>
-      <c r="B39" s="5" t="n"/>
+      <c r="B39" s="4" t="n"/>
       <c r="C39" s="5" t="n"/>
       <c r="D39" s="5" t="n"/>
       <c r="E39" s="5" t="n"/>
@@ -1007,10 +1047,11 @@
       <c r="I39" s="5" t="n"/>
       <c r="J39" s="5" t="n"/>
       <c r="K39" s="5" t="n"/>
+      <c r="L39" s="5" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="4" t="n"/>
-      <c r="B40" s="5" t="n"/>
+      <c r="B40" s="4" t="n"/>
       <c r="C40" s="5" t="n"/>
       <c r="D40" s="5" t="n"/>
       <c r="E40" s="5" t="n"/>
@@ -1020,10 +1061,11 @@
       <c r="I40" s="5" t="n"/>
       <c r="J40" s="5" t="n"/>
       <c r="K40" s="5" t="n"/>
+      <c r="L40" s="5" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="4" t="n"/>
-      <c r="B41" s="5" t="n"/>
+      <c r="B41" s="4" t="n"/>
       <c r="C41" s="5" t="n"/>
       <c r="D41" s="5" t="n"/>
       <c r="E41" s="5" t="n"/>
@@ -1033,10 +1075,11 @@
       <c r="I41" s="5" t="n"/>
       <c r="J41" s="5" t="n"/>
       <c r="K41" s="5" t="n"/>
+      <c r="L41" s="5" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="4" t="n"/>
-      <c r="B42" s="5" t="n"/>
+      <c r="B42" s="4" t="n"/>
       <c r="C42" s="5" t="n"/>
       <c r="D42" s="5" t="n"/>
       <c r="E42" s="5" t="n"/>
@@ -1046,10 +1089,11 @@
       <c r="I42" s="5" t="n"/>
       <c r="J42" s="5" t="n"/>
       <c r="K42" s="5" t="n"/>
+      <c r="L42" s="5" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="n"/>
-      <c r="B43" s="5" t="n"/>
+      <c r="B43" s="4" t="n"/>
       <c r="C43" s="5" t="n"/>
       <c r="D43" s="5" t="n"/>
       <c r="E43" s="5" t="n"/>
@@ -1059,10 +1103,11 @@
       <c r="I43" s="5" t="n"/>
       <c r="J43" s="5" t="n"/>
       <c r="K43" s="5" t="n"/>
+      <c r="L43" s="5" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="n"/>
-      <c r="B44" s="5" t="n"/>
+      <c r="B44" s="4" t="n"/>
       <c r="C44" s="5" t="n"/>
       <c r="D44" s="5" t="n"/>
       <c r="E44" s="5" t="n"/>
@@ -1072,10 +1117,11 @@
       <c r="I44" s="5" t="n"/>
       <c r="J44" s="5" t="n"/>
       <c r="K44" s="5" t="n"/>
+      <c r="L44" s="5" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="4" t="n"/>
-      <c r="B45" s="5" t="n"/>
+      <c r="B45" s="4" t="n"/>
       <c r="C45" s="5" t="n"/>
       <c r="D45" s="5" t="n"/>
       <c r="E45" s="5" t="n"/>
@@ -1085,10 +1131,11 @@
       <c r="I45" s="5" t="n"/>
       <c r="J45" s="5" t="n"/>
       <c r="K45" s="5" t="n"/>
+      <c r="L45" s="5" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="4" t="n"/>
-      <c r="B46" s="5" t="n"/>
+      <c r="B46" s="4" t="n"/>
       <c r="C46" s="5" t="n"/>
       <c r="D46" s="5" t="n"/>
       <c r="E46" s="5" t="n"/>
@@ -1098,10 +1145,11 @@
       <c r="I46" s="5" t="n"/>
       <c r="J46" s="5" t="n"/>
       <c r="K46" s="5" t="n"/>
+      <c r="L46" s="5" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="4" t="n"/>
-      <c r="B47" s="5" t="n"/>
+      <c r="B47" s="4" t="n"/>
       <c r="C47" s="5" t="n"/>
       <c r="D47" s="5" t="n"/>
       <c r="E47" s="5" t="n"/>
@@ -1111,10 +1159,11 @@
       <c r="I47" s="5" t="n"/>
       <c r="J47" s="5" t="n"/>
       <c r="K47" s="5" t="n"/>
+      <c r="L47" s="5" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="4" t="n"/>
-      <c r="B48" s="5" t="n"/>
+      <c r="B48" s="4" t="n"/>
       <c r="C48" s="5" t="n"/>
       <c r="D48" s="5" t="n"/>
       <c r="E48" s="5" t="n"/>
@@ -1124,10 +1173,11 @@
       <c r="I48" s="5" t="n"/>
       <c r="J48" s="5" t="n"/>
       <c r="K48" s="5" t="n"/>
+      <c r="L48" s="5" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="4" t="n"/>
-      <c r="B49" s="5" t="n"/>
+      <c r="B49" s="4" t="n"/>
       <c r="C49" s="5" t="n"/>
       <c r="D49" s="5" t="n"/>
       <c r="E49" s="5" t="n"/>
@@ -1137,10 +1187,11 @@
       <c r="I49" s="5" t="n"/>
       <c r="J49" s="5" t="n"/>
       <c r="K49" s="5" t="n"/>
+      <c r="L49" s="5" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="4" t="n"/>
-      <c r="B50" s="5" t="n"/>
+      <c r="B50" s="4" t="n"/>
       <c r="C50" s="5" t="n"/>
       <c r="D50" s="5" t="n"/>
       <c r="E50" s="5" t="n"/>
@@ -1150,10 +1201,11 @@
       <c r="I50" s="5" t="n"/>
       <c r="J50" s="5" t="n"/>
       <c r="K50" s="5" t="n"/>
+      <c r="L50" s="5" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="4" t="n"/>
-      <c r="B51" s="5" t="n"/>
+      <c r="B51" s="4" t="n"/>
       <c r="C51" s="5" t="n"/>
       <c r="D51" s="5" t="n"/>
       <c r="E51" s="5" t="n"/>
@@ -1163,10 +1215,11 @@
       <c r="I51" s="5" t="n"/>
       <c r="J51" s="5" t="n"/>
       <c r="K51" s="5" t="n"/>
+      <c r="L51" s="5" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="4" t="n"/>
-      <c r="B52" s="5" t="n"/>
+      <c r="B52" s="4" t="n"/>
       <c r="C52" s="5" t="n"/>
       <c r="D52" s="5" t="n"/>
       <c r="E52" s="5" t="n"/>
@@ -1176,10 +1229,11 @@
       <c r="I52" s="5" t="n"/>
       <c r="J52" s="5" t="n"/>
       <c r="K52" s="5" t="n"/>
+      <c r="L52" s="5" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="4" t="n"/>
-      <c r="B53" s="5" t="n"/>
+      <c r="B53" s="4" t="n"/>
       <c r="C53" s="5" t="n"/>
       <c r="D53" s="5" t="n"/>
       <c r="E53" s="5" t="n"/>
@@ -1189,10 +1243,11 @@
       <c r="I53" s="5" t="n"/>
       <c r="J53" s="5" t="n"/>
       <c r="K53" s="5" t="n"/>
+      <c r="L53" s="5" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="4" t="n"/>
-      <c r="B54" s="5" t="n"/>
+      <c r="B54" s="4" t="n"/>
       <c r="C54" s="5" t="n"/>
       <c r="D54" s="5" t="n"/>
       <c r="E54" s="5" t="n"/>
@@ -1202,10 +1257,11 @@
       <c r="I54" s="5" t="n"/>
       <c r="J54" s="5" t="n"/>
       <c r="K54" s="5" t="n"/>
+      <c r="L54" s="5" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="4" t="n"/>
-      <c r="B55" s="5" t="n"/>
+      <c r="B55" s="4" t="n"/>
       <c r="C55" s="5" t="n"/>
       <c r="D55" s="5" t="n"/>
       <c r="E55" s="5" t="n"/>
@@ -1215,10 +1271,11 @@
       <c r="I55" s="5" t="n"/>
       <c r="J55" s="5" t="n"/>
       <c r="K55" s="5" t="n"/>
+      <c r="L55" s="5" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="4" t="n"/>
-      <c r="B56" s="5" t="n"/>
+      <c r="B56" s="4" t="n"/>
       <c r="C56" s="5" t="n"/>
       <c r="D56" s="5" t="n"/>
       <c r="E56" s="5" t="n"/>
@@ -1228,10 +1285,11 @@
       <c r="I56" s="5" t="n"/>
       <c r="J56" s="5" t="n"/>
       <c r="K56" s="5" t="n"/>
+      <c r="L56" s="5" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="4" t="n"/>
-      <c r="B57" s="5" t="n"/>
+      <c r="B57" s="4" t="n"/>
       <c r="C57" s="5" t="n"/>
       <c r="D57" s="5" t="n"/>
       <c r="E57" s="5" t="n"/>
@@ -1241,10 +1299,11 @@
       <c r="I57" s="5" t="n"/>
       <c r="J57" s="5" t="n"/>
       <c r="K57" s="5" t="n"/>
+      <c r="L57" s="5" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="4" t="n"/>
-      <c r="B58" s="5" t="n"/>
+      <c r="B58" s="4" t="n"/>
       <c r="C58" s="5" t="n"/>
       <c r="D58" s="5" t="n"/>
       <c r="E58" s="5" t="n"/>
@@ -1254,10 +1313,11 @@
       <c r="I58" s="5" t="n"/>
       <c r="J58" s="5" t="n"/>
       <c r="K58" s="5" t="n"/>
+      <c r="L58" s="5" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="4" t="n"/>
-      <c r="B59" s="5" t="n"/>
+      <c r="B59" s="4" t="n"/>
       <c r="C59" s="5" t="n"/>
       <c r="D59" s="5" t="n"/>
       <c r="E59" s="5" t="n"/>
@@ -1267,10 +1327,11 @@
       <c r="I59" s="5" t="n"/>
       <c r="J59" s="5" t="n"/>
       <c r="K59" s="5" t="n"/>
+      <c r="L59" s="5" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="4" t="n"/>
-      <c r="B60" s="5" t="n"/>
+      <c r="B60" s="4" t="n"/>
       <c r="C60" s="5" t="n"/>
       <c r="D60" s="5" t="n"/>
       <c r="E60" s="5" t="n"/>
@@ -1280,10 +1341,11 @@
       <c r="I60" s="5" t="n"/>
       <c r="J60" s="5" t="n"/>
       <c r="K60" s="5" t="n"/>
+      <c r="L60" s="5" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="4" t="n"/>
-      <c r="B61" s="5" t="n"/>
+      <c r="B61" s="4" t="n"/>
       <c r="C61" s="5" t="n"/>
       <c r="D61" s="5" t="n"/>
       <c r="E61" s="5" t="n"/>
@@ -1293,10 +1355,11 @@
       <c r="I61" s="5" t="n"/>
       <c r="J61" s="5" t="n"/>
       <c r="K61" s="5" t="n"/>
+      <c r="L61" s="5" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="4" t="n"/>
-      <c r="B62" s="5" t="n"/>
+      <c r="B62" s="4" t="n"/>
       <c r="C62" s="5" t="n"/>
       <c r="D62" s="5" t="n"/>
       <c r="E62" s="5" t="n"/>
@@ -1306,10 +1369,11 @@
       <c r="I62" s="5" t="n"/>
       <c r="J62" s="5" t="n"/>
       <c r="K62" s="5" t="n"/>
+      <c r="L62" s="5" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="4" t="n"/>
-      <c r="B63" s="5" t="n"/>
+      <c r="B63" s="4" t="n"/>
       <c r="C63" s="5" t="n"/>
       <c r="D63" s="5" t="n"/>
       <c r="E63" s="5" t="n"/>
@@ -1319,10 +1383,11 @@
       <c r="I63" s="5" t="n"/>
       <c r="J63" s="5" t="n"/>
       <c r="K63" s="5" t="n"/>
+      <c r="L63" s="5" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="4" t="n"/>
-      <c r="B64" s="5" t="n"/>
+      <c r="B64" s="4" t="n"/>
       <c r="C64" s="5" t="n"/>
       <c r="D64" s="5" t="n"/>
       <c r="E64" s="5" t="n"/>
@@ -1332,10 +1397,11 @@
       <c r="I64" s="5" t="n"/>
       <c r="J64" s="5" t="n"/>
       <c r="K64" s="5" t="n"/>
+      <c r="L64" s="5" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="4" t="n"/>
-      <c r="B65" s="5" t="n"/>
+      <c r="B65" s="4" t="n"/>
       <c r="C65" s="5" t="n"/>
       <c r="D65" s="5" t="n"/>
       <c r="E65" s="5" t="n"/>
@@ -1345,10 +1411,11 @@
       <c r="I65" s="5" t="n"/>
       <c r="J65" s="5" t="n"/>
       <c r="K65" s="5" t="n"/>
+      <c r="L65" s="5" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="4" t="n"/>
-      <c r="B66" s="5" t="n"/>
+      <c r="B66" s="4" t="n"/>
       <c r="C66" s="5" t="n"/>
       <c r="D66" s="5" t="n"/>
       <c r="E66" s="5" t="n"/>
@@ -1358,10 +1425,11 @@
       <c r="I66" s="5" t="n"/>
       <c r="J66" s="5" t="n"/>
       <c r="K66" s="5" t="n"/>
+      <c r="L66" s="5" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="4" t="n"/>
-      <c r="B67" s="5" t="n"/>
+      <c r="B67" s="4" t="n"/>
       <c r="C67" s="5" t="n"/>
       <c r="D67" s="5" t="n"/>
       <c r="E67" s="5" t="n"/>
@@ -1371,10 +1439,11 @@
       <c r="I67" s="5" t="n"/>
       <c r="J67" s="5" t="n"/>
       <c r="K67" s="5" t="n"/>
+      <c r="L67" s="5" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="4" t="n"/>
-      <c r="B68" s="5" t="n"/>
+      <c r="B68" s="4" t="n"/>
       <c r="C68" s="5" t="n"/>
       <c r="D68" s="5" t="n"/>
       <c r="E68" s="5" t="n"/>
@@ -1384,10 +1453,11 @@
       <c r="I68" s="5" t="n"/>
       <c r="J68" s="5" t="n"/>
       <c r="K68" s="5" t="n"/>
+      <c r="L68" s="5" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="4" t="n"/>
-      <c r="B69" s="5" t="n"/>
+      <c r="B69" s="4" t="n"/>
       <c r="C69" s="5" t="n"/>
       <c r="D69" s="5" t="n"/>
       <c r="E69" s="5" t="n"/>
@@ -1397,10 +1467,11 @@
       <c r="I69" s="5" t="n"/>
       <c r="J69" s="5" t="n"/>
       <c r="K69" s="5" t="n"/>
+      <c r="L69" s="5" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="4" t="n"/>
-      <c r="B70" s="5" t="n"/>
+      <c r="B70" s="4" t="n"/>
       <c r="C70" s="5" t="n"/>
       <c r="D70" s="5" t="n"/>
       <c r="E70" s="5" t="n"/>
@@ -1410,10 +1481,11 @@
       <c r="I70" s="5" t="n"/>
       <c r="J70" s="5" t="n"/>
       <c r="K70" s="5" t="n"/>
+      <c r="L70" s="5" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="4" t="n"/>
-      <c r="B71" s="5" t="n"/>
+      <c r="B71" s="4" t="n"/>
       <c r="C71" s="5" t="n"/>
       <c r="D71" s="5" t="n"/>
       <c r="E71" s="5" t="n"/>
@@ -1423,10 +1495,11 @@
       <c r="I71" s="5" t="n"/>
       <c r="J71" s="5" t="n"/>
       <c r="K71" s="5" t="n"/>
+      <c r="L71" s="5" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="4" t="n"/>
-      <c r="B72" s="5" t="n"/>
+      <c r="B72" s="4" t="n"/>
       <c r="C72" s="5" t="n"/>
       <c r="D72" s="5" t="n"/>
       <c r="E72" s="5" t="n"/>
@@ -1436,10 +1509,11 @@
       <c r="I72" s="5" t="n"/>
       <c r="J72" s="5" t="n"/>
       <c r="K72" s="5" t="n"/>
+      <c r="L72" s="5" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="4" t="n"/>
-      <c r="B73" s="5" t="n"/>
+      <c r="B73" s="4" t="n"/>
       <c r="C73" s="5" t="n"/>
       <c r="D73" s="5" t="n"/>
       <c r="E73" s="5" t="n"/>
@@ -1449,10 +1523,11 @@
       <c r="I73" s="5" t="n"/>
       <c r="J73" s="5" t="n"/>
       <c r="K73" s="5" t="n"/>
+      <c r="L73" s="5" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="4" t="n"/>
-      <c r="B74" s="5" t="n"/>
+      <c r="B74" s="4" t="n"/>
       <c r="C74" s="5" t="n"/>
       <c r="D74" s="5" t="n"/>
       <c r="E74" s="5" t="n"/>
@@ -1462,10 +1537,11 @@
       <c r="I74" s="5" t="n"/>
       <c r="J74" s="5" t="n"/>
       <c r="K74" s="5" t="n"/>
+      <c r="L74" s="5" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="4" t="n"/>
-      <c r="B75" s="5" t="n"/>
+      <c r="B75" s="4" t="n"/>
       <c r="C75" s="5" t="n"/>
       <c r="D75" s="5" t="n"/>
       <c r="E75" s="5" t="n"/>
@@ -1475,10 +1551,11 @@
       <c r="I75" s="5" t="n"/>
       <c r="J75" s="5" t="n"/>
       <c r="K75" s="5" t="n"/>
+      <c r="L75" s="5" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="4" t="n"/>
-      <c r="B76" s="5" t="n"/>
+      <c r="B76" s="4" t="n"/>
       <c r="C76" s="5" t="n"/>
       <c r="D76" s="5" t="n"/>
       <c r="E76" s="5" t="n"/>
@@ -1488,10 +1565,11 @@
       <c r="I76" s="5" t="n"/>
       <c r="J76" s="5" t="n"/>
       <c r="K76" s="5" t="n"/>
+      <c r="L76" s="5" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="4" t="n"/>
-      <c r="B77" s="5" t="n"/>
+      <c r="B77" s="4" t="n"/>
       <c r="C77" s="5" t="n"/>
       <c r="D77" s="5" t="n"/>
       <c r="E77" s="5" t="n"/>
@@ -1501,10 +1579,11 @@
       <c r="I77" s="5" t="n"/>
       <c r="J77" s="5" t="n"/>
       <c r="K77" s="5" t="n"/>
+      <c r="L77" s="5" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="4" t="n"/>
-      <c r="B78" s="5" t="n"/>
+      <c r="B78" s="4" t="n"/>
       <c r="C78" s="5" t="n"/>
       <c r="D78" s="5" t="n"/>
       <c r="E78" s="5" t="n"/>
@@ -1514,10 +1593,11 @@
       <c r="I78" s="5" t="n"/>
       <c r="J78" s="5" t="n"/>
       <c r="K78" s="5" t="n"/>
+      <c r="L78" s="5" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="4" t="n"/>
-      <c r="B79" s="5" t="n"/>
+      <c r="B79" s="4" t="n"/>
       <c r="C79" s="5" t="n"/>
       <c r="D79" s="5" t="n"/>
       <c r="E79" s="5" t="n"/>
@@ -1527,10 +1607,11 @@
       <c r="I79" s="5" t="n"/>
       <c r="J79" s="5" t="n"/>
       <c r="K79" s="5" t="n"/>
+      <c r="L79" s="5" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="4" t="n"/>
-      <c r="B80" s="5" t="n"/>
+      <c r="B80" s="4" t="n"/>
       <c r="C80" s="5" t="n"/>
       <c r="D80" s="5" t="n"/>
       <c r="E80" s="5" t="n"/>
@@ -1540,10 +1621,11 @@
       <c r="I80" s="5" t="n"/>
       <c r="J80" s="5" t="n"/>
       <c r="K80" s="5" t="n"/>
+      <c r="L80" s="5" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="4" t="n"/>
-      <c r="B81" s="5" t="n"/>
+      <c r="B81" s="4" t="n"/>
       <c r="C81" s="5" t="n"/>
       <c r="D81" s="5" t="n"/>
       <c r="E81" s="5" t="n"/>
@@ -1553,10 +1635,11 @@
       <c r="I81" s="5" t="n"/>
       <c r="J81" s="5" t="n"/>
       <c r="K81" s="5" t="n"/>
+      <c r="L81" s="5" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="4" t="n"/>
-      <c r="B82" s="5" t="n"/>
+      <c r="B82" s="4" t="n"/>
       <c r="C82" s="5" t="n"/>
       <c r="D82" s="5" t="n"/>
       <c r="E82" s="5" t="n"/>
@@ -1566,10 +1649,11 @@
       <c r="I82" s="5" t="n"/>
       <c r="J82" s="5" t="n"/>
       <c r="K82" s="5" t="n"/>
+      <c r="L82" s="5" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="4" t="n"/>
-      <c r="B83" s="5" t="n"/>
+      <c r="B83" s="4" t="n"/>
       <c r="C83" s="5" t="n"/>
       <c r="D83" s="5" t="n"/>
       <c r="E83" s="5" t="n"/>
@@ -1579,10 +1663,11 @@
       <c r="I83" s="5" t="n"/>
       <c r="J83" s="5" t="n"/>
       <c r="K83" s="5" t="n"/>
+      <c r="L83" s="5" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="4" t="n"/>
-      <c r="B84" s="5" t="n"/>
+      <c r="B84" s="4" t="n"/>
       <c r="C84" s="5" t="n"/>
       <c r="D84" s="5" t="n"/>
       <c r="E84" s="5" t="n"/>
@@ -1592,10 +1677,11 @@
       <c r="I84" s="5" t="n"/>
       <c r="J84" s="5" t="n"/>
       <c r="K84" s="5" t="n"/>
+      <c r="L84" s="5" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="4" t="n"/>
-      <c r="B85" s="5" t="n"/>
+      <c r="B85" s="4" t="n"/>
       <c r="C85" s="5" t="n"/>
       <c r="D85" s="5" t="n"/>
       <c r="E85" s="5" t="n"/>
@@ -1605,10 +1691,11 @@
       <c r="I85" s="5" t="n"/>
       <c r="J85" s="5" t="n"/>
       <c r="K85" s="5" t="n"/>
+      <c r="L85" s="5" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="4" t="n"/>
-      <c r="B86" s="5" t="n"/>
+      <c r="B86" s="4" t="n"/>
       <c r="C86" s="5" t="n"/>
       <c r="D86" s="5" t="n"/>
       <c r="E86" s="5" t="n"/>
@@ -1618,10 +1705,11 @@
       <c r="I86" s="5" t="n"/>
       <c r="J86" s="5" t="n"/>
       <c r="K86" s="5" t="n"/>
+      <c r="L86" s="5" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="4" t="n"/>
-      <c r="B87" s="5" t="n"/>
+      <c r="B87" s="4" t="n"/>
       <c r="C87" s="5" t="n"/>
       <c r="D87" s="5" t="n"/>
       <c r="E87" s="5" t="n"/>
@@ -1631,10 +1719,11 @@
       <c r="I87" s="5" t="n"/>
       <c r="J87" s="5" t="n"/>
       <c r="K87" s="5" t="n"/>
+      <c r="L87" s="5" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="4" t="n"/>
-      <c r="B88" s="5" t="n"/>
+      <c r="B88" s="4" t="n"/>
       <c r="C88" s="5" t="n"/>
       <c r="D88" s="5" t="n"/>
       <c r="E88" s="5" t="n"/>
@@ -1644,10 +1733,11 @@
       <c r="I88" s="5" t="n"/>
       <c r="J88" s="5" t="n"/>
       <c r="K88" s="5" t="n"/>
+      <c r="L88" s="5" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="4" t="n"/>
-      <c r="B89" s="5" t="n"/>
+      <c r="B89" s="4" t="n"/>
       <c r="C89" s="5" t="n"/>
       <c r="D89" s="5" t="n"/>
       <c r="E89" s="5" t="n"/>
@@ -1657,10 +1747,11 @@
       <c r="I89" s="5" t="n"/>
       <c r="J89" s="5" t="n"/>
       <c r="K89" s="5" t="n"/>
+      <c r="L89" s="5" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="4" t="n"/>
-      <c r="B90" s="5" t="n"/>
+      <c r="B90" s="4" t="n"/>
       <c r="C90" s="5" t="n"/>
       <c r="D90" s="5" t="n"/>
       <c r="E90" s="5" t="n"/>
@@ -1670,10 +1761,11 @@
       <c r="I90" s="5" t="n"/>
       <c r="J90" s="5" t="n"/>
       <c r="K90" s="5" t="n"/>
+      <c r="L90" s="5" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="4" t="n"/>
-      <c r="B91" s="5" t="n"/>
+      <c r="B91" s="4" t="n"/>
       <c r="C91" s="5" t="n"/>
       <c r="D91" s="5" t="n"/>
       <c r="E91" s="5" t="n"/>
@@ -1683,10 +1775,11 @@
       <c r="I91" s="5" t="n"/>
       <c r="J91" s="5" t="n"/>
       <c r="K91" s="5" t="n"/>
+      <c r="L91" s="5" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="4" t="n"/>
-      <c r="B92" s="5" t="n"/>
+      <c r="B92" s="4" t="n"/>
       <c r="C92" s="5" t="n"/>
       <c r="D92" s="5" t="n"/>
       <c r="E92" s="5" t="n"/>
@@ -1696,10 +1789,11 @@
       <c r="I92" s="5" t="n"/>
       <c r="J92" s="5" t="n"/>
       <c r="K92" s="5" t="n"/>
+      <c r="L92" s="5" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="4" t="n"/>
-      <c r="B93" s="5" t="n"/>
+      <c r="B93" s="4" t="n"/>
       <c r="C93" s="5" t="n"/>
       <c r="D93" s="5" t="n"/>
       <c r="E93" s="5" t="n"/>
@@ -1709,10 +1803,11 @@
       <c r="I93" s="5" t="n"/>
       <c r="J93" s="5" t="n"/>
       <c r="K93" s="5" t="n"/>
+      <c r="L93" s="5" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="4" t="n"/>
-      <c r="B94" s="5" t="n"/>
+      <c r="B94" s="4" t="n"/>
       <c r="C94" s="5" t="n"/>
       <c r="D94" s="5" t="n"/>
       <c r="E94" s="5" t="n"/>
@@ -1722,10 +1817,11 @@
       <c r="I94" s="5" t="n"/>
       <c r="J94" s="5" t="n"/>
       <c r="K94" s="5" t="n"/>
+      <c r="L94" s="5" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="4" t="n"/>
-      <c r="B95" s="5" t="n"/>
+      <c r="B95" s="4" t="n"/>
       <c r="C95" s="5" t="n"/>
       <c r="D95" s="5" t="n"/>
       <c r="E95" s="5" t="n"/>
@@ -1735,10 +1831,11 @@
       <c r="I95" s="5" t="n"/>
       <c r="J95" s="5" t="n"/>
       <c r="K95" s="5" t="n"/>
+      <c r="L95" s="5" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="4" t="n"/>
-      <c r="B96" s="5" t="n"/>
+      <c r="B96" s="4" t="n"/>
       <c r="C96" s="5" t="n"/>
       <c r="D96" s="5" t="n"/>
       <c r="E96" s="5" t="n"/>
@@ -1748,10 +1845,11 @@
       <c r="I96" s="5" t="n"/>
       <c r="J96" s="5" t="n"/>
       <c r="K96" s="5" t="n"/>
+      <c r="L96" s="5" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="4" t="n"/>
-      <c r="B97" s="5" t="n"/>
+      <c r="B97" s="4" t="n"/>
       <c r="C97" s="5" t="n"/>
       <c r="D97" s="5" t="n"/>
       <c r="E97" s="5" t="n"/>
@@ -1761,10 +1859,11 @@
       <c r="I97" s="5" t="n"/>
       <c r="J97" s="5" t="n"/>
       <c r="K97" s="5" t="n"/>
+      <c r="L97" s="5" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="4" t="n"/>
-      <c r="B98" s="5" t="n"/>
+      <c r="B98" s="4" t="n"/>
       <c r="C98" s="5" t="n"/>
       <c r="D98" s="5" t="n"/>
       <c r="E98" s="5" t="n"/>
@@ -1774,10 +1873,11 @@
       <c r="I98" s="5" t="n"/>
       <c r="J98" s="5" t="n"/>
       <c r="K98" s="5" t="n"/>
+      <c r="L98" s="5" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="4" t="n"/>
-      <c r="B99" s="5" t="n"/>
+      <c r="B99" s="4" t="n"/>
       <c r="C99" s="5" t="n"/>
       <c r="D99" s="5" t="n"/>
       <c r="E99" s="5" t="n"/>
@@ -1787,10 +1887,11 @@
       <c r="I99" s="5" t="n"/>
       <c r="J99" s="5" t="n"/>
       <c r="K99" s="5" t="n"/>
+      <c r="L99" s="5" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="4" t="n"/>
-      <c r="B100" s="5" t="n"/>
+      <c r="B100" s="4" t="n"/>
       <c r="C100" s="5" t="n"/>
       <c r="D100" s="5" t="n"/>
       <c r="E100" s="5" t="n"/>
@@ -1800,10 +1901,11 @@
       <c r="I100" s="5" t="n"/>
       <c r="J100" s="5" t="n"/>
       <c r="K100" s="5" t="n"/>
+      <c r="L100" s="5" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="4" t="n"/>
-      <c r="B101" s="5" t="n"/>
+      <c r="B101" s="4" t="n"/>
       <c r="C101" s="5" t="n"/>
       <c r="D101" s="5" t="n"/>
       <c r="E101" s="5" t="n"/>
@@ -1813,10 +1915,11 @@
       <c r="I101" s="5" t="n"/>
       <c r="J101" s="5" t="n"/>
       <c r="K101" s="5" t="n"/>
+      <c r="L101" s="5" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="4" t="n"/>
-      <c r="B102" s="5" t="n"/>
+      <c r="B102" s="4" t="n"/>
       <c r="C102" s="5" t="n"/>
       <c r="D102" s="5" t="n"/>
       <c r="E102" s="5" t="n"/>
@@ -1826,10 +1929,11 @@
       <c r="I102" s="5" t="n"/>
       <c r="J102" s="5" t="n"/>
       <c r="K102" s="5" t="n"/>
+      <c r="L102" s="5" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="4" t="n"/>
-      <c r="B103" s="5" t="n"/>
+      <c r="B103" s="4" t="n"/>
       <c r="C103" s="5" t="n"/>
       <c r="D103" s="5" t="n"/>
       <c r="E103" s="5" t="n"/>
@@ -1839,10 +1943,11 @@
       <c r="I103" s="5" t="n"/>
       <c r="J103" s="5" t="n"/>
       <c r="K103" s="5" t="n"/>
+      <c r="L103" s="5" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="4" t="n"/>
-      <c r="B104" s="5" t="n"/>
+      <c r="B104" s="4" t="n"/>
       <c r="C104" s="5" t="n"/>
       <c r="D104" s="5" t="n"/>
       <c r="E104" s="5" t="n"/>
@@ -1852,10 +1957,11 @@
       <c r="I104" s="5" t="n"/>
       <c r="J104" s="5" t="n"/>
       <c r="K104" s="5" t="n"/>
+      <c r="L104" s="5" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="4" t="n"/>
-      <c r="B105" s="5" t="n"/>
+      <c r="B105" s="4" t="n"/>
       <c r="C105" s="5" t="n"/>
       <c r="D105" s="5" t="n"/>
       <c r="E105" s="5" t="n"/>
@@ -1865,10 +1971,11 @@
       <c r="I105" s="5" t="n"/>
       <c r="J105" s="5" t="n"/>
       <c r="K105" s="5" t="n"/>
+      <c r="L105" s="5" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="4" t="n"/>
-      <c r="B106" s="5" t="n"/>
+      <c r="B106" s="4" t="n"/>
       <c r="C106" s="5" t="n"/>
       <c r="D106" s="5" t="n"/>
       <c r="E106" s="5" t="n"/>
@@ -1878,10 +1985,11 @@
       <c r="I106" s="5" t="n"/>
       <c r="J106" s="5" t="n"/>
       <c r="K106" s="5" t="n"/>
+      <c r="L106" s="5" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="4" t="n"/>
-      <c r="B107" s="5" t="n"/>
+      <c r="B107" s="4" t="n"/>
       <c r="C107" s="5" t="n"/>
       <c r="D107" s="5" t="n"/>
       <c r="E107" s="5" t="n"/>
@@ -1891,10 +1999,11 @@
       <c r="I107" s="5" t="n"/>
       <c r="J107" s="5" t="n"/>
       <c r="K107" s="5" t="n"/>
+      <c r="L107" s="5" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="4" t="n"/>
-      <c r="B108" s="5" t="n"/>
+      <c r="B108" s="4" t="n"/>
       <c r="C108" s="5" t="n"/>
       <c r="D108" s="5" t="n"/>
       <c r="E108" s="5" t="n"/>
@@ -1904,10 +2013,11 @@
       <c r="I108" s="5" t="n"/>
       <c r="J108" s="5" t="n"/>
       <c r="K108" s="5" t="n"/>
+      <c r="L108" s="5" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="4" t="n"/>
-      <c r="B109" s="5" t="n"/>
+      <c r="B109" s="4" t="n"/>
       <c r="C109" s="5" t="n"/>
       <c r="D109" s="5" t="n"/>
       <c r="E109" s="5" t="n"/>
@@ -1917,10 +2027,11 @@
       <c r="I109" s="5" t="n"/>
       <c r="J109" s="5" t="n"/>
       <c r="K109" s="5" t="n"/>
+      <c r="L109" s="5" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="4" t="n"/>
-      <c r="B110" s="5" t="n"/>
+      <c r="B110" s="4" t="n"/>
       <c r="C110" s="5" t="n"/>
       <c r="D110" s="5" t="n"/>
       <c r="E110" s="5" t="n"/>
@@ -1930,10 +2041,11 @@
       <c r="I110" s="5" t="n"/>
       <c r="J110" s="5" t="n"/>
       <c r="K110" s="5" t="n"/>
+      <c r="L110" s="5" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="4" t="n"/>
-      <c r="B111" s="5" t="n"/>
+      <c r="B111" s="4" t="n"/>
       <c r="C111" s="5" t="n"/>
       <c r="D111" s="5" t="n"/>
       <c r="E111" s="5" t="n"/>
@@ -1943,10 +2055,11 @@
       <c r="I111" s="5" t="n"/>
       <c r="J111" s="5" t="n"/>
       <c r="K111" s="5" t="n"/>
+      <c r="L111" s="5" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="4" t="n"/>
-      <c r="B112" s="5" t="n"/>
+      <c r="B112" s="4" t="n"/>
       <c r="C112" s="5" t="n"/>
       <c r="D112" s="5" t="n"/>
       <c r="E112" s="5" t="n"/>
@@ -1956,10 +2069,11 @@
       <c r="I112" s="5" t="n"/>
       <c r="J112" s="5" t="n"/>
       <c r="K112" s="5" t="n"/>
+      <c r="L112" s="5" t="n"/>
     </row>
     <row r="113">
       <c r="A113" s="4" t="n"/>
-      <c r="B113" s="5" t="n"/>
+      <c r="B113" s="4" t="n"/>
       <c r="C113" s="5" t="n"/>
       <c r="D113" s="5" t="n"/>
       <c r="E113" s="5" t="n"/>
@@ -1969,10 +2083,11 @@
       <c r="I113" s="5" t="n"/>
       <c r="J113" s="5" t="n"/>
       <c r="K113" s="5" t="n"/>
+      <c r="L113" s="5" t="n"/>
     </row>
     <row r="114">
       <c r="A114" s="4" t="n"/>
-      <c r="B114" s="5" t="n"/>
+      <c r="B114" s="4" t="n"/>
       <c r="C114" s="5" t="n"/>
       <c r="D114" s="5" t="n"/>
       <c r="E114" s="5" t="n"/>
@@ -1982,10 +2097,11 @@
       <c r="I114" s="5" t="n"/>
       <c r="J114" s="5" t="n"/>
       <c r="K114" s="5" t="n"/>
+      <c r="L114" s="5" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="4" t="n"/>
-      <c r="B115" s="5" t="n"/>
+      <c r="B115" s="4" t="n"/>
       <c r="C115" s="5" t="n"/>
       <c r="D115" s="5" t="n"/>
       <c r="E115" s="5" t="n"/>
@@ -1995,10 +2111,11 @@
       <c r="I115" s="5" t="n"/>
       <c r="J115" s="5" t="n"/>
       <c r="K115" s="5" t="n"/>
+      <c r="L115" s="5" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="4" t="n"/>
-      <c r="B116" s="5" t="n"/>
+      <c r="B116" s="4" t="n"/>
       <c r="C116" s="5" t="n"/>
       <c r="D116" s="5" t="n"/>
       <c r="E116" s="5" t="n"/>
@@ -2008,10 +2125,11 @@
       <c r="I116" s="5" t="n"/>
       <c r="J116" s="5" t="n"/>
       <c r="K116" s="5" t="n"/>
+      <c r="L116" s="5" t="n"/>
     </row>
     <row r="117">
       <c r="A117" s="4" t="n"/>
-      <c r="B117" s="5" t="n"/>
+      <c r="B117" s="4" t="n"/>
       <c r="C117" s="5" t="n"/>
       <c r="D117" s="5" t="n"/>
       <c r="E117" s="5" t="n"/>
@@ -2021,10 +2139,11 @@
       <c r="I117" s="5" t="n"/>
       <c r="J117" s="5" t="n"/>
       <c r="K117" s="5" t="n"/>
+      <c r="L117" s="5" t="n"/>
     </row>
     <row r="118">
       <c r="A118" s="4" t="n"/>
-      <c r="B118" s="5" t="n"/>
+      <c r="B118" s="4" t="n"/>
       <c r="C118" s="5" t="n"/>
       <c r="D118" s="5" t="n"/>
       <c r="E118" s="5" t="n"/>
@@ -2034,10 +2153,11 @@
       <c r="I118" s="5" t="n"/>
       <c r="J118" s="5" t="n"/>
       <c r="K118" s="5" t="n"/>
+      <c r="L118" s="5" t="n"/>
     </row>
     <row r="119">
       <c r="A119" s="4" t="n"/>
-      <c r="B119" s="5" t="n"/>
+      <c r="B119" s="4" t="n"/>
       <c r="C119" s="5" t="n"/>
       <c r="D119" s="5" t="n"/>
       <c r="E119" s="5" t="n"/>
@@ -2047,10 +2167,11 @@
       <c r="I119" s="5" t="n"/>
       <c r="J119" s="5" t="n"/>
       <c r="K119" s="5" t="n"/>
+      <c r="L119" s="5" t="n"/>
     </row>
     <row r="120">
       <c r="A120" s="4" t="n"/>
-      <c r="B120" s="5" t="n"/>
+      <c r="B120" s="4" t="n"/>
       <c r="C120" s="5" t="n"/>
       <c r="D120" s="5" t="n"/>
       <c r="E120" s="5" t="n"/>
@@ -2060,10 +2181,11 @@
       <c r="I120" s="5" t="n"/>
       <c r="J120" s="5" t="n"/>
       <c r="K120" s="5" t="n"/>
+      <c r="L120" s="5" t="n"/>
     </row>
     <row r="121">
       <c r="A121" s="4" t="n"/>
-      <c r="B121" s="5" t="n"/>
+      <c r="B121" s="4" t="n"/>
       <c r="C121" s="5" t="n"/>
       <c r="D121" s="5" t="n"/>
       <c r="E121" s="5" t="n"/>
@@ -2073,10 +2195,11 @@
       <c r="I121" s="5" t="n"/>
       <c r="J121" s="5" t="n"/>
       <c r="K121" s="5" t="n"/>
+      <c r="L121" s="5" t="n"/>
     </row>
     <row r="122">
       <c r="A122" s="4" t="n"/>
-      <c r="B122" s="5" t="n"/>
+      <c r="B122" s="4" t="n"/>
       <c r="C122" s="5" t="n"/>
       <c r="D122" s="5" t="n"/>
       <c r="E122" s="5" t="n"/>
@@ -2086,10 +2209,11 @@
       <c r="I122" s="5" t="n"/>
       <c r="J122" s="5" t="n"/>
       <c r="K122" s="5" t="n"/>
+      <c r="L122" s="5" t="n"/>
     </row>
     <row r="123">
       <c r="A123" s="4" t="n"/>
-      <c r="B123" s="5" t="n"/>
+      <c r="B123" s="4" t="n"/>
       <c r="C123" s="5" t="n"/>
       <c r="D123" s="5" t="n"/>
       <c r="E123" s="5" t="n"/>
@@ -2099,10 +2223,11 @@
       <c r="I123" s="5" t="n"/>
       <c r="J123" s="5" t="n"/>
       <c r="K123" s="5" t="n"/>
+      <c r="L123" s="5" t="n"/>
     </row>
     <row r="124">
       <c r="A124" s="4" t="n"/>
-      <c r="B124" s="5" t="n"/>
+      <c r="B124" s="4" t="n"/>
       <c r="C124" s="5" t="n"/>
       <c r="D124" s="5" t="n"/>
       <c r="E124" s="5" t="n"/>
@@ -2112,10 +2237,11 @@
       <c r="I124" s="5" t="n"/>
       <c r="J124" s="5" t="n"/>
       <c r="K124" s="5" t="n"/>
+      <c r="L124" s="5" t="n"/>
     </row>
     <row r="125">
       <c r="A125" s="4" t="n"/>
-      <c r="B125" s="5" t="n"/>
+      <c r="B125" s="4" t="n"/>
       <c r="C125" s="5" t="n"/>
       <c r="D125" s="5" t="n"/>
       <c r="E125" s="5" t="n"/>
@@ -2125,10 +2251,11 @@
       <c r="I125" s="5" t="n"/>
       <c r="J125" s="5" t="n"/>
       <c r="K125" s="5" t="n"/>
+      <c r="L125" s="5" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="4" t="n"/>
-      <c r="B126" s="5" t="n"/>
+      <c r="B126" s="4" t="n"/>
       <c r="C126" s="5" t="n"/>
       <c r="D126" s="5" t="n"/>
       <c r="E126" s="5" t="n"/>
@@ -2138,10 +2265,11 @@
       <c r="I126" s="5" t="n"/>
       <c r="J126" s="5" t="n"/>
       <c r="K126" s="5" t="n"/>
+      <c r="L126" s="5" t="n"/>
     </row>
     <row r="127">
       <c r="A127" s="4" t="n"/>
-      <c r="B127" s="5" t="n"/>
+      <c r="B127" s="4" t="n"/>
       <c r="C127" s="5" t="n"/>
       <c r="D127" s="5" t="n"/>
       <c r="E127" s="5" t="n"/>
@@ -2151,10 +2279,11 @@
       <c r="I127" s="5" t="n"/>
       <c r="J127" s="5" t="n"/>
       <c r="K127" s="5" t="n"/>
+      <c r="L127" s="5" t="n"/>
     </row>
     <row r="128">
       <c r="A128" s="4" t="n"/>
-      <c r="B128" s="5" t="n"/>
+      <c r="B128" s="4" t="n"/>
       <c r="C128" s="5" t="n"/>
       <c r="D128" s="5" t="n"/>
       <c r="E128" s="5" t="n"/>
@@ -2164,10 +2293,11 @@
       <c r="I128" s="5" t="n"/>
       <c r="J128" s="5" t="n"/>
       <c r="K128" s="5" t="n"/>
+      <c r="L128" s="5" t="n"/>
     </row>
     <row r="129">
       <c r="A129" s="4" t="n"/>
-      <c r="B129" s="5" t="n"/>
+      <c r="B129" s="4" t="n"/>
       <c r="C129" s="5" t="n"/>
       <c r="D129" s="5" t="n"/>
       <c r="E129" s="5" t="n"/>
@@ -2177,10 +2307,11 @@
       <c r="I129" s="5" t="n"/>
       <c r="J129" s="5" t="n"/>
       <c r="K129" s="5" t="n"/>
+      <c r="L129" s="5" t="n"/>
     </row>
     <row r="130">
       <c r="A130" s="4" t="n"/>
-      <c r="B130" s="5" t="n"/>
+      <c r="B130" s="4" t="n"/>
       <c r="C130" s="5" t="n"/>
       <c r="D130" s="5" t="n"/>
       <c r="E130" s="5" t="n"/>
@@ -2190,10 +2321,11 @@
       <c r="I130" s="5" t="n"/>
       <c r="J130" s="5" t="n"/>
       <c r="K130" s="5" t="n"/>
+      <c r="L130" s="5" t="n"/>
     </row>
     <row r="131">
       <c r="A131" s="4" t="n"/>
-      <c r="B131" s="5" t="n"/>
+      <c r="B131" s="4" t="n"/>
       <c r="C131" s="5" t="n"/>
       <c r="D131" s="5" t="n"/>
       <c r="E131" s="5" t="n"/>
@@ -2203,10 +2335,11 @@
       <c r="I131" s="5" t="n"/>
       <c r="J131" s="5" t="n"/>
       <c r="K131" s="5" t="n"/>
+      <c r="L131" s="5" t="n"/>
     </row>
     <row r="132">
       <c r="A132" s="4" t="n"/>
-      <c r="B132" s="5" t="n"/>
+      <c r="B132" s="4" t="n"/>
       <c r="C132" s="5" t="n"/>
       <c r="D132" s="5" t="n"/>
       <c r="E132" s="5" t="n"/>
@@ -2216,10 +2349,11 @@
       <c r="I132" s="5" t="n"/>
       <c r="J132" s="5" t="n"/>
       <c r="K132" s="5" t="n"/>
+      <c r="L132" s="5" t="n"/>
     </row>
     <row r="133">
       <c r="A133" s="4" t="n"/>
-      <c r="B133" s="5" t="n"/>
+      <c r="B133" s="4" t="n"/>
       <c r="C133" s="5" t="n"/>
       <c r="D133" s="5" t="n"/>
       <c r="E133" s="5" t="n"/>
@@ -2229,10 +2363,11 @@
       <c r="I133" s="5" t="n"/>
       <c r="J133" s="5" t="n"/>
       <c r="K133" s="5" t="n"/>
+      <c r="L133" s="5" t="n"/>
     </row>
     <row r="134">
       <c r="A134" s="4" t="n"/>
-      <c r="B134" s="5" t="n"/>
+      <c r="B134" s="4" t="n"/>
       <c r="C134" s="5" t="n"/>
       <c r="D134" s="5" t="n"/>
       <c r="E134" s="5" t="n"/>
@@ -2242,10 +2377,11 @@
       <c r="I134" s="5" t="n"/>
       <c r="J134" s="5" t="n"/>
       <c r="K134" s="5" t="n"/>
+      <c r="L134" s="5" t="n"/>
     </row>
     <row r="135">
       <c r="A135" s="4" t="n"/>
-      <c r="B135" s="5" t="n"/>
+      <c r="B135" s="4" t="n"/>
       <c r="C135" s="5" t="n"/>
       <c r="D135" s="5" t="n"/>
       <c r="E135" s="5" t="n"/>
@@ -2255,10 +2391,11 @@
       <c r="I135" s="5" t="n"/>
       <c r="J135" s="5" t="n"/>
       <c r="K135" s="5" t="n"/>
+      <c r="L135" s="5" t="n"/>
     </row>
     <row r="136">
       <c r="A136" s="4" t="n"/>
-      <c r="B136" s="5" t="n"/>
+      <c r="B136" s="4" t="n"/>
       <c r="C136" s="5" t="n"/>
       <c r="D136" s="5" t="n"/>
       <c r="E136" s="5" t="n"/>
@@ -2268,10 +2405,11 @@
       <c r="I136" s="5" t="n"/>
       <c r="J136" s="5" t="n"/>
       <c r="K136" s="5" t="n"/>
+      <c r="L136" s="5" t="n"/>
     </row>
     <row r="137">
       <c r="A137" s="4" t="n"/>
-      <c r="B137" s="5" t="n"/>
+      <c r="B137" s="4" t="n"/>
       <c r="C137" s="5" t="n"/>
       <c r="D137" s="5" t="n"/>
       <c r="E137" s="5" t="n"/>
@@ -2281,10 +2419,11 @@
       <c r="I137" s="5" t="n"/>
       <c r="J137" s="5" t="n"/>
       <c r="K137" s="5" t="n"/>
+      <c r="L137" s="5" t="n"/>
     </row>
     <row r="138">
       <c r="A138" s="4" t="n"/>
-      <c r="B138" s="5" t="n"/>
+      <c r="B138" s="4" t="n"/>
       <c r="C138" s="5" t="n"/>
       <c r="D138" s="5" t="n"/>
       <c r="E138" s="5" t="n"/>
@@ -2294,10 +2433,11 @@
       <c r="I138" s="5" t="n"/>
       <c r="J138" s="5" t="n"/>
       <c r="K138" s="5" t="n"/>
+      <c r="L138" s="5" t="n"/>
     </row>
     <row r="139">
       <c r="A139" s="4" t="n"/>
-      <c r="B139" s="5" t="n"/>
+      <c r="B139" s="4" t="n"/>
       <c r="C139" s="5" t="n"/>
       <c r="D139" s="5" t="n"/>
       <c r="E139" s="5" t="n"/>
@@ -2307,10 +2447,11 @@
       <c r="I139" s="5" t="n"/>
       <c r="J139" s="5" t="n"/>
       <c r="K139" s="5" t="n"/>
+      <c r="L139" s="5" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="4" t="n"/>
-      <c r="B140" s="5" t="n"/>
+      <c r="B140" s="4" t="n"/>
       <c r="C140" s="5" t="n"/>
       <c r="D140" s="5" t="n"/>
       <c r="E140" s="5" t="n"/>
@@ -2320,10 +2461,11 @@
       <c r="I140" s="5" t="n"/>
       <c r="J140" s="5" t="n"/>
       <c r="K140" s="5" t="n"/>
+      <c r="L140" s="5" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="4" t="n"/>
-      <c r="B141" s="5" t="n"/>
+      <c r="B141" s="4" t="n"/>
       <c r="C141" s="5" t="n"/>
       <c r="D141" s="5" t="n"/>
       <c r="E141" s="5" t="n"/>
@@ -2333,10 +2475,11 @@
       <c r="I141" s="5" t="n"/>
       <c r="J141" s="5" t="n"/>
       <c r="K141" s="5" t="n"/>
+      <c r="L141" s="5" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="4" t="n"/>
-      <c r="B142" s="5" t="n"/>
+      <c r="B142" s="4" t="n"/>
       <c r="C142" s="5" t="n"/>
       <c r="D142" s="5" t="n"/>
       <c r="E142" s="5" t="n"/>
@@ -2346,10 +2489,11 @@
       <c r="I142" s="5" t="n"/>
       <c r="J142" s="5" t="n"/>
       <c r="K142" s="5" t="n"/>
+      <c r="L142" s="5" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="4" t="n"/>
-      <c r="B143" s="5" t="n"/>
+      <c r="B143" s="4" t="n"/>
       <c r="C143" s="5" t="n"/>
       <c r="D143" s="5" t="n"/>
       <c r="E143" s="5" t="n"/>
@@ -2359,10 +2503,11 @@
       <c r="I143" s="5" t="n"/>
       <c r="J143" s="5" t="n"/>
       <c r="K143" s="5" t="n"/>
+      <c r="L143" s="5" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="4" t="n"/>
-      <c r="B144" s="5" t="n"/>
+      <c r="B144" s="4" t="n"/>
       <c r="C144" s="5" t="n"/>
       <c r="D144" s="5" t="n"/>
       <c r="E144" s="5" t="n"/>
@@ -2372,10 +2517,11 @@
       <c r="I144" s="5" t="n"/>
       <c r="J144" s="5" t="n"/>
       <c r="K144" s="5" t="n"/>
+      <c r="L144" s="5" t="n"/>
     </row>
     <row r="145">
       <c r="A145" s="4" t="n"/>
-      <c r="B145" s="5" t="n"/>
+      <c r="B145" s="4" t="n"/>
       <c r="C145" s="5" t="n"/>
       <c r="D145" s="5" t="n"/>
       <c r="E145" s="5" t="n"/>
@@ -2385,10 +2531,11 @@
       <c r="I145" s="5" t="n"/>
       <c r="J145" s="5" t="n"/>
       <c r="K145" s="5" t="n"/>
+      <c r="L145" s="5" t="n"/>
     </row>
     <row r="146">
       <c r="A146" s="4" t="n"/>
-      <c r="B146" s="5" t="n"/>
+      <c r="B146" s="4" t="n"/>
       <c r="C146" s="5" t="n"/>
       <c r="D146" s="5" t="n"/>
       <c r="E146" s="5" t="n"/>
@@ -2398,10 +2545,11 @@
       <c r="I146" s="5" t="n"/>
       <c r="J146" s="5" t="n"/>
       <c r="K146" s="5" t="n"/>
+      <c r="L146" s="5" t="n"/>
     </row>
     <row r="147">
       <c r="A147" s="4" t="n"/>
-      <c r="B147" s="5" t="n"/>
+      <c r="B147" s="4" t="n"/>
       <c r="C147" s="5" t="n"/>
       <c r="D147" s="5" t="n"/>
       <c r="E147" s="5" t="n"/>
@@ -2411,10 +2559,11 @@
       <c r="I147" s="5" t="n"/>
       <c r="J147" s="5" t="n"/>
       <c r="K147" s="5" t="n"/>
+      <c r="L147" s="5" t="n"/>
     </row>
     <row r="148">
       <c r="A148" s="4" t="n"/>
-      <c r="B148" s="5" t="n"/>
+      <c r="B148" s="4" t="n"/>
       <c r="C148" s="5" t="n"/>
       <c r="D148" s="5" t="n"/>
       <c r="E148" s="5" t="n"/>
@@ -2424,10 +2573,11 @@
       <c r="I148" s="5" t="n"/>
       <c r="J148" s="5" t="n"/>
       <c r="K148" s="5" t="n"/>
+      <c r="L148" s="5" t="n"/>
     </row>
     <row r="149">
       <c r="A149" s="4" t="n"/>
-      <c r="B149" s="5" t="n"/>
+      <c r="B149" s="4" t="n"/>
       <c r="C149" s="5" t="n"/>
       <c r="D149" s="5" t="n"/>
       <c r="E149" s="5" t="n"/>
@@ -2437,10 +2587,11 @@
       <c r="I149" s="5" t="n"/>
       <c r="J149" s="5" t="n"/>
       <c r="K149" s="5" t="n"/>
+      <c r="L149" s="5" t="n"/>
     </row>
     <row r="150">
       <c r="A150" s="4" t="n"/>
-      <c r="B150" s="5" t="n"/>
+      <c r="B150" s="4" t="n"/>
       <c r="C150" s="5" t="n"/>
       <c r="D150" s="5" t="n"/>
       <c r="E150" s="5" t="n"/>
@@ -2450,10 +2601,11 @@
       <c r="I150" s="5" t="n"/>
       <c r="J150" s="5" t="n"/>
       <c r="K150" s="5" t="n"/>
+      <c r="L150" s="5" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="4" t="n"/>
-      <c r="B151" s="5" t="n"/>
+      <c r="B151" s="4" t="n"/>
       <c r="C151" s="5" t="n"/>
       <c r="D151" s="5" t="n"/>
       <c r="E151" s="5" t="n"/>
@@ -2463,10 +2615,11 @@
       <c r="I151" s="5" t="n"/>
       <c r="J151" s="5" t="n"/>
       <c r="K151" s="5" t="n"/>
+      <c r="L151" s="5" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="4" t="n"/>
-      <c r="B152" s="5" t="n"/>
+      <c r="B152" s="4" t="n"/>
       <c r="C152" s="5" t="n"/>
       <c r="D152" s="5" t="n"/>
       <c r="E152" s="5" t="n"/>
@@ -2476,10 +2629,11 @@
       <c r="I152" s="5" t="n"/>
       <c r="J152" s="5" t="n"/>
       <c r="K152" s="5" t="n"/>
+      <c r="L152" s="5" t="n"/>
     </row>
     <row r="153">
       <c r="A153" s="4" t="n"/>
-      <c r="B153" s="5" t="n"/>
+      <c r="B153" s="4" t="n"/>
       <c r="C153" s="5" t="n"/>
       <c r="D153" s="5" t="n"/>
       <c r="E153" s="5" t="n"/>
@@ -2489,10 +2643,11 @@
       <c r="I153" s="5" t="n"/>
       <c r="J153" s="5" t="n"/>
       <c r="K153" s="5" t="n"/>
+      <c r="L153" s="5" t="n"/>
     </row>
     <row r="154">
       <c r="A154" s="4" t="n"/>
-      <c r="B154" s="5" t="n"/>
+      <c r="B154" s="4" t="n"/>
       <c r="C154" s="5" t="n"/>
       <c r="D154" s="5" t="n"/>
       <c r="E154" s="5" t="n"/>
@@ -2502,19 +2657,20 @@
       <c r="I154" s="5" t="n"/>
       <c r="J154" s="5" t="n"/>
       <c r="K154" s="5" t="n"/>
+      <c r="L154" s="5" t="n"/>
     </row>
     <row r="156">
       <c r="A156" s="6" t="inlineStr">
         <is>
-          <t>💡 Astuce : Remplissez les noms en colonne A et les disponibilités (0 ou 1) dans les autres colonnes</t>
+          <t>💡 Astuce : Remplissez prénom/nom en colonnes A et B, puis les disponibilités (0 ou 1) dans les colonnes P1 à P10</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A156:K156"/>
+    <mergeCell ref="A156:L156"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>